<commit_message>
fix made in GST project
</commit_message>
<xml_diff>
--- a/target/test-classes/GSTProject/GSTPROJECT/Interview1.xlsx
+++ b/target/test-classes/GSTProject/GSTPROJECT/Interview1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="81">
   <si>
     <t>TestCase</t>
   </si>
@@ -58,19 +58,227 @@
   </si>
   <si>
     <t>xpath</t>
+  </si>
+  <si>
+    <t>ADVCLICK</t>
+  </si>
+  <si>
+    <t>case3</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>case4</t>
+  </si>
+  <si>
+    <t>invoice</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>case5</t>
+  </si>
+  <si>
+    <t>case6</t>
+  </si>
+  <si>
+    <t>knowmore</t>
+  </si>
+  <si>
+    <t>case7</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>case8</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>case9</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>case10</t>
+  </si>
+  <si>
+    <t>WINDOW</t>
+  </si>
+  <si>
+    <t>case11</t>
+  </si>
+  <si>
+    <t>case12</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>case13</t>
+  </si>
+  <si>
+    <t>case14</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>case15</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>case16</t>
+  </si>
+  <si>
+    <t>partner</t>
+  </si>
+  <si>
+    <t>case17</t>
+  </si>
+  <si>
+    <t>vendors</t>
+  </si>
+  <si>
+    <t>case18</t>
+  </si>
+  <si>
+    <t>tendors</t>
+  </si>
+  <si>
+    <t>case19</t>
+  </si>
+  <si>
+    <t>case20</t>
+  </si>
+  <si>
+    <t>case21</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>case22</t>
+  </si>
+  <si>
+    <t>SETTEXT</t>
+  </si>
+  <si>
+    <t>organisation</t>
+  </si>
+  <si>
+    <t>ABC Private Limited</t>
+  </si>
+  <si>
+    <t>case23</t>
+  </si>
+  <si>
+    <t>www.ABC.com</t>
+  </si>
+  <si>
+    <t>case24</t>
+  </si>
+  <si>
+    <t>gstid</t>
+  </si>
+  <si>
+    <t>case25</t>
+  </si>
+  <si>
+    <t>turnover</t>
+  </si>
+  <si>
+    <t>case26</t>
+  </si>
+  <si>
+    <t>profit</t>
+  </si>
+  <si>
+    <t>blacklist</t>
+  </si>
+  <si>
+    <t>case28</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>case27</t>
+  </si>
+  <si>
+    <t>case29</t>
+  </si>
+  <si>
+    <t>alert</t>
+  </si>
+  <si>
+    <t>case30</t>
+  </si>
+  <si>
+    <t>case31</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>GST option</t>
+  </si>
+  <si>
+    <t>Invoice option</t>
+  </si>
+  <si>
+    <t>Next button</t>
+  </si>
+  <si>
+    <t>Stats option</t>
+  </si>
+  <si>
+    <t>LinkedIN option</t>
+  </si>
+  <si>
+    <t>Login option</t>
+  </si>
+  <si>
+    <t>Media option</t>
+  </si>
+  <si>
+    <t>Partner option</t>
+  </si>
+  <si>
+    <t>Inputting text</t>
+  </si>
+  <si>
+    <t>JCLICK</t>
+  </si>
+  <si>
+    <t>video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,13 +298,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -389,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -401,7 +616,7 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -448,32 +663,834 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="2">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E34" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>